<commit_message>
add idea to challenge
</commit_message>
<xml_diff>
--- a/src/main/java/resources1/testdataQA.xlsx
+++ b/src/main/java/resources1/testdataQA.xlsx
@@ -1,22 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20379"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Engy.Moghazy\eclipse-workspace2forGIT\Ideate\src\main\java\resources1\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3442D2E6-5039-4F41-BACC-0444F765CD64}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{6F6F657D-F877-43BD-BE39-5D2B57079878}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11265" windowHeight="3870" activeTab="1" xr2:uid="{F67B910A-3901-4799-A5C0-097D62FF54E1}"/>
+    <workbookView xWindow="1116" yWindow="1116" windowWidth="17280" windowHeight="8964" xr2:uid="{F67B910A-3901-4799-A5C0-097D62FF54E1}"/>
   </bookViews>
   <sheets>
     <sheet name="employee" sheetId="1" r:id="rId1"/>
     <sheet name="superadmin" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:G8"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -66,7 +62,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -74,7 +70,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -438,14 +434,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCCBF0E5-7CA2-4722-92CD-158A06AF9A10}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="51.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="42.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="51.8984375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="42.3984375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -489,14 +485,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D94FB6A0-FDE4-49ED-8917-B42EB2E1F0BC}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.42578125" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" customWidth="1"/>
+    <col min="1" max="1" width="30.3984375" customWidth="1"/>
+    <col min="2" max="2" width="19.8984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>